<commit_message>
par reveille manifestement recorrection de boundsduration 1812eb569ca95d9a35720021efd59649a1ad48f7
</commit_message>
<xml_diff>
--- a/VoitureBalaisDecisions/ig/StructureDefinition-FrRangeMedication.xlsx
+++ b/VoitureBalaisDecisions/ig/StructureDefinition-FrRangeMedication.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="119">
   <si>
     <t>Property</t>
   </si>
@@ -42,7 +42,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Range with UCUM or EDQM quantity units</t>
+    <t>Range with UCUM or EDQM codes if code is used</t>
   </si>
   <si>
     <t>Status</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-12T16:52:42+00:00</t>
+    <t>2025-08-13T14:10:49+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Range with low and high unit UCUM or EDQM encoded</t>
+    <t>Range with low and high unit UCUM or EDQM codes if code is used</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -253,13 +253,13 @@
 </t>
   </si>
   <si>
-    <t>Set of values bounded by precise low and high fixed quantity (no comparator) with UCUM or EDQM unit</t>
-  </si>
-  <si>
-    <t>A set of ordered Quantities defined by a precise low and high limit defined by a fixed quantity (no comparator) with UCUM or EDQM unit</t>
-  </si>
-  <si>
-    <t>The stated low and high value are assumed to have arbitrarily high precision when it comes to determining which values are in the range. I.e. 1.99 is not in the range 2 -&gt; 3. Low and high limit are precisely defined, no element 'comparator' in the simpleQuantity defining each bound. The limits are defined by a fixed quantity (no comparator) with UCUM unit.</t>
+    <t>Set of values bounded by precise low and high fixed quantity (no comparator)</t>
+  </si>
+  <si>
+    <t>A set of ordered Quantities defined by a precise low and high limit defined by a fixed quantity (no comparator)</t>
+  </si>
+  <si>
+    <t>The stated low and high value are assumed to have arbitrarily high precision when it comes to determining which values are in the range. I.e. 1.99 is not in the range 2 -&gt; 3. Low and high limit are precisely defined, no element 'comparator' in the simpleQuantity defining each bound. The limits are defined by a fixed quantity (no comparator).</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1
@@ -345,16 +345,13 @@
 </t>
   </si>
   <si>
-    <t>low bound with UCUM or EDQM unit</t>
-  </si>
-  <si>
-    <t>unit of measure SHALL be UCUM or EDQM encoded</t>
+    <t>Low limit</t>
+  </si>
+  <si>
+    <t>The low limit. The boundary is inclusive.</t>
   </si>
   <si>
     <t>If the low element is missing, the low boundary is not known.</t>
-  </si>
-  <si>
-    <t>force UCUM or EDQM unit encoding</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
@@ -370,7 +367,10 @@
     <t>Range.high</t>
   </si>
   <si>
-    <t>high bound with UCUM or EDQM unit</t>
+    <t>High limit</t>
+  </si>
+  <si>
+    <t>The high limit. The boundary is inclusive.</t>
   </si>
   <si>
     <t>If the high element is missing, the high boundary is not known.</t>
@@ -707,7 +707,7 @@
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="28.80859375" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.4296875" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
@@ -1209,9 +1209,7 @@
       <c r="N5" t="s" s="2">
         <v>109</v>
       </c>
-      <c r="O5" t="s" s="2">
-        <v>110</v>
-      </c>
+      <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
         <v>75</v>
       </c>
@@ -1271,21 +1269,21 @@
         <v>75</v>
       </c>
       <c r="AJ5" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AK5" t="s" s="2">
         <v>111</v>
       </c>
-      <c r="AK5" t="s" s="2">
+      <c r="AL5" t="s" s="2">
         <v>112</v>
-      </c>
-      <c r="AL5" t="s" s="2">
-        <v>113</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
@@ -1311,17 +1309,15 @@
         <v>106</v>
       </c>
       <c r="L6" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="M6" t="s" s="2">
         <v>115</v>
-      </c>
-      <c r="M6" t="s" s="2">
-        <v>108</v>
       </c>
       <c r="N6" t="s" s="2">
         <v>116</v>
       </c>
-      <c r="O6" t="s" s="2">
-        <v>110</v>
-      </c>
+      <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
         <v>75</v>
       </c>
@@ -1369,7 +1365,7 @@
         <v>75</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AG6" t="s" s="2">
         <v>76</v>
@@ -1381,7 +1377,7 @@
         <v>75</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AK6" t="s" s="2">
         <v>117</v>

</xml_diff>